<commit_message>
Change metadata templates and add INS
</commit_message>
<xml_diff>
--- a/example/NHANES-2017-2018/STR-NHANES-2017-2018.xlsx
+++ b/example/NHANES-2017-2018/STR-NHANES-2017-2018.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="InfoSheet" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="FILESTREAM" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="MESSAGESTREAM" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="MESSAGETOPIC" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="InfoSheet" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="FILESTREAM" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="MESSAGESTREAM" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="MESSAGETOPIC" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t xml:space="preserve">Property </t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Study_ID</t>
   </si>
   <si>
-    <t xml:space="preserve">NHANES-2017-2018</t>
+    <t xml:space="preserve">nhanes:/STL1740399181578561</t>
   </si>
   <si>
     <t xml:space="preserve">Version</t>
@@ -79,13 +79,13 @@
     <t xml:space="preserve">NHANES-2017-2018-DEMO_J</t>
   </si>
   <si>
-    <t xml:space="preserve">NHANES-DEMO</t>
+    <t xml:space="preserve">nhanes:/SDDICT1740398910528131</t>
   </si>
   <si>
     <t xml:space="preserve">nhanes:DPL-DMQ_J-QUESTIONNAIRE</t>
   </si>
   <si>
-    <t xml:space="preserve">example@example.com</t>
+    <t xml:space="preserve">admin@example.com</t>
   </si>
   <si>
     <t xml:space="preserve">Public</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">NHANES-2017-2018-TCHOL_J</t>
   </si>
   <si>
-    <t xml:space="preserve">NHANES-LAB-RESULTS</t>
+    <t xml:space="preserve">nhanes:/SDDICT1740398928689521</t>
   </si>
   <si>
     <t xml:space="preserve">nhanes:DPL-ROCHE-HITACHI-COBAS-6000-ANALYZER</t>
@@ -127,7 +127,10 @@
     <t xml:space="preserve">NHANES-2017-2018-DPQ_J</t>
   </si>
   <si>
-    <t xml:space="preserve">NHANES-DPQ</t>
+    <t xml:space="preserve">nhanes:/SDDICT1740398947916601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nhanes:DPL-DPQ_J-QUESTIONNAIRE</t>
   </si>
   <si>
     <t xml:space="preserve">hasURI</t>
@@ -182,12 +185,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -198,6 +195,12 @@
       <u val="single"/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -263,24 +266,24 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -288,20 +291,28 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -317,21 +328,127 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="11.5"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="8.83"/>
   </cols>
@@ -351,7 +468,7 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3"/>
@@ -442,14 +559,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -487,14 +604,14 @@
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -502,17 +619,17 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -520,17 +637,17 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -538,17 +655,17 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -556,17 +673,17 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -574,17 +691,17 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -592,30 +709,48 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="C9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
     </row>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -626,13 +761,14 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="example@example.com"/>
-    <hyperlink ref="E3" r:id="rId2" display="example@example.com"/>
-    <hyperlink ref="E4" r:id="rId3" display="example@example.com"/>
-    <hyperlink ref="E5" r:id="rId4" display="example@example.com"/>
-    <hyperlink ref="E6" r:id="rId5" display="example@example.com"/>
-    <hyperlink ref="E7" r:id="rId6" display="example@example.com"/>
-    <hyperlink ref="E8" r:id="rId7" display="example@example.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="admin@example.com"/>
+    <hyperlink ref="E3" r:id="rId2" display="admin@example.com"/>
+    <hyperlink ref="E4" r:id="rId3" display="admin@example.com"/>
+    <hyperlink ref="E5" r:id="rId4" display="admin@example.com"/>
+    <hyperlink ref="E6" r:id="rId5" display="admin@example.com"/>
+    <hyperlink ref="E7" r:id="rId6" display="admin@example.com"/>
+    <hyperlink ref="E8" r:id="rId7" display="admin@example.com"/>
+    <hyperlink ref="E9" r:id="rId8" display="admin@example.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -645,7 +781,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -663,22 +799,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>15</v>
@@ -789,13 +925,13 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -807,10 +943,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>13</v>

</xml_diff>